<commit_message>
CDD_Buzzer.docx edited with commented CDD_RL.xlsx issues
</commit_message>
<xml_diff>
--- a/Workspace/Design/CDD_RL.xlsx
+++ b/Workspace/Design/CDD_RL.xlsx
@@ -1,20 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18431"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="N:\software\Air-Conditioner-Screen-Team-4\Workspace\Design\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ismail samy\Desktop\GIT\Workspace\Design\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{DF811D2A-C044-4567-AB87-2B1FE9F5B071}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8196" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
+  <externalReferences>
+    <externalReference r:id="rId3"/>
+  </externalReferences>
   <calcPr calcId="0" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
@@ -25,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="32">
   <si>
     <t>Air Conditioner Screen Review Log</t>
   </si>
@@ -106,12 +110,27 @@
   </si>
   <si>
     <t>RV_4</t>
+  </si>
+  <si>
+    <t>RV_5</t>
+  </si>
+  <si>
+    <t>CDD_LCD Dynamic Design</t>
+  </si>
+  <si>
+    <t>CDD_LCD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Saber Osamn </t>
+  </si>
+  <si>
+    <t xml:space="preserve">section 4.1(mode management) missing, section 4.2(sequence diagram)missing, shared resources describe if needed or no ! And protection section, sec 6.2 and 6.3 (link time, post build) franko arabic not accebtable </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="m/d/yyyy"/>
   </numFmts>
@@ -218,11 +237,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -268,6 +284,10 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -351,6 +371,19 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Sheet1"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0" refreshError="1"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -649,363 +682,378 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AMK34"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:G6"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.42578125" style="2" customWidth="1"/>
-    <col min="2" max="2" width="44.5703125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="23.5703125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="18.28515625" style="2" customWidth="1"/>
-    <col min="5" max="5" width="26" style="2" customWidth="1"/>
-    <col min="6" max="6" width="76.7109375" style="2" customWidth="1"/>
-    <col min="7" max="1025" width="14.42578125" style="2" customWidth="1"/>
+    <col min="1" max="1" width="14.44140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="44.5546875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="23.5546875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="18.33203125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="26" style="1" customWidth="1"/>
+    <col min="6" max="6" width="76.6640625" style="1" customWidth="1"/>
+    <col min="7" max="1025" width="14.44140625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-    </row>
-    <row r="2" spans="1:7" s="5" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="3" t="s">
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
+      <c r="G1" s="20"/>
+    </row>
+    <row r="2" spans="1:7" s="4" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="F2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="G2" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="D3" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="7" t="s">
+      <c r="E3" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="F3" s="6" t="s">
+      <c r="F3" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="G3" s="8" t="s">
+      <c r="G3" s="7" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
+    <row r="4" spans="1:7" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="9" t="s">
+      <c r="B4" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="C4" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="E4" s="10" t="s">
+      <c r="D4" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="F4" s="11" t="s">
+      <c r="F4" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="G4" s="11" t="s">
+      <c r="G4" s="10" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:7" s="10" customFormat="1" ht="27" x14ac:dyDescent="0.2">
-      <c r="A5" s="6" t="s">
+    <row r="5" spans="1:7" s="9" customFormat="1" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="C5" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="D5" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="E5" s="7" t="s">
+      <c r="D5" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="F5" s="17" t="s">
+      <c r="F5" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="G5" s="8" t="s">
+      <c r="G5" s="7" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:7" s="10" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A6" s="6" t="s">
+    <row r="6" spans="1:7" s="9" customFormat="1" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="B6" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="C6" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="D6" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="E6" s="18" t="s">
+      <c r="D6" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E6" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="F6" s="19" t="s">
+      <c r="F6" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="G6" s="20">
+      <c r="G6" s="19">
         <v>43210</v>
       </c>
     </row>
-    <row r="7" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="6"/>
-      <c r="B7" s="6"/>
-      <c r="C7" s="6"/>
-      <c r="D7" s="6" t="s">
+    <row r="7" spans="1:7" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="G7" s="21">
+        <v>43210</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="5"/>
+      <c r="B8" s="5"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="5" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="6"/>
-      <c r="B8" s="6"/>
-      <c r="C8" s="6"/>
-      <c r="D8" s="6" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="6"/>
-      <c r="B9" s="6"/>
-      <c r="C9" s="6"/>
-      <c r="D9" s="6" t="s">
+    <row r="9" spans="1:7" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="5"/>
+      <c r="B9" s="5"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="5" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="6"/>
-      <c r="B10" s="6"/>
-      <c r="C10" s="6"/>
-      <c r="D10" s="6" t="s">
+    <row r="10" spans="1:7" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="5"/>
+      <c r="B10" s="5"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="5" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="6"/>
-      <c r="B11" s="7"/>
-      <c r="C11" s="6"/>
-      <c r="D11" s="6" t="s">
+    <row r="11" spans="1:7" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="5"/>
+      <c r="B11" s="6"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="5" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:7" s="12" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="13" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="6"/>
-      <c r="B13" s="13"/>
-      <c r="C13" s="6"/>
-      <c r="D13" s="6" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="6"/>
-      <c r="B14" s="13"/>
-      <c r="C14" s="6"/>
-      <c r="D14" s="6" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" s="10" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="6"/>
-      <c r="B15" s="13"/>
-      <c r="C15" s="6"/>
-      <c r="D15" s="6" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" s="10" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="6"/>
-      <c r="B16" s="13"/>
-      <c r="C16" s="6"/>
-      <c r="D16" s="6" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" s="10" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="6"/>
-      <c r="B17" s="13"/>
-      <c r="C17" s="6"/>
-      <c r="D17" s="6" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="6"/>
-      <c r="B18" s="13"/>
-      <c r="C18" s="6"/>
-      <c r="D18" s="6" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="6"/>
-      <c r="B19" s="13"/>
-      <c r="C19" s="6"/>
-      <c r="D19" s="6" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="6"/>
-      <c r="B20" s="13"/>
-      <c r="C20" s="6"/>
-      <c r="D20" s="6" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="6"/>
-      <c r="B21" s="13"/>
-      <c r="C21" s="6"/>
-      <c r="D21" s="6" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" s="10" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="6"/>
-      <c r="B22" s="13"/>
-      <c r="C22" s="6"/>
-      <c r="D22" s="6" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="6"/>
-      <c r="B23" s="13"/>
-      <c r="C23" s="6"/>
-      <c r="D23" s="6" t="s">
+    <row r="12" spans="1:7" s="11" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="1:7" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="5"/>
+      <c r="B13" s="12"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="5"/>
+      <c r="B14" s="12"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" s="9" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="5"/>
+      <c r="B15" s="12"/>
+      <c r="C15" s="5"/>
+      <c r="D15" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" s="9" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="5"/>
+      <c r="B16" s="12"/>
+      <c r="C16" s="5"/>
+      <c r="D16" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" s="9" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="5"/>
+      <c r="B17" s="12"/>
+      <c r="C17" s="5"/>
+      <c r="D17" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="5"/>
+      <c r="B18" s="12"/>
+      <c r="C18" s="5"/>
+      <c r="D18" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="5"/>
+      <c r="B19" s="12"/>
+      <c r="C19" s="5"/>
+      <c r="D19" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="5"/>
+      <c r="B20" s="12"/>
+      <c r="C20" s="5"/>
+      <c r="D20" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="5"/>
+      <c r="B21" s="12"/>
+      <c r="C21" s="5"/>
+      <c r="D21" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" s="9" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="5"/>
+      <c r="B22" s="12"/>
+      <c r="C22" s="5"/>
+      <c r="D22" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="5"/>
+      <c r="B23" s="12"/>
+      <c r="C23" s="5"/>
+      <c r="D23" s="5" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="24" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="6"/>
-      <c r="B24" s="13"/>
-      <c r="C24" s="6"/>
-      <c r="D24" s="6" t="s">
+    <row r="24" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="5"/>
+      <c r="B24" s="12"/>
+      <c r="C24" s="5"/>
+      <c r="D24" s="5" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="25" spans="1:4" s="10" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="6"/>
-      <c r="B25" s="13"/>
-      <c r="C25" s="6"/>
-      <c r="D25" s="6" t="s">
+    <row r="25" spans="1:4" s="9" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="5"/>
+      <c r="B25" s="12"/>
+      <c r="C25" s="5"/>
+      <c r="D25" s="5" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="26" spans="1:4" s="10" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="6"/>
-      <c r="B26" s="13"/>
-      <c r="C26" s="6"/>
-      <c r="D26" s="6" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" s="10" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="6"/>
-      <c r="B27" s="13"/>
-      <c r="C27" s="6"/>
-      <c r="D27" s="6" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="6"/>
-      <c r="B28" s="13"/>
-      <c r="C28" s="6"/>
-      <c r="D28" s="6" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="6"/>
-      <c r="B29" s="13"/>
-      <c r="C29" s="6"/>
-      <c r="D29" s="6" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="31" spans="1:4" s="10" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="15"/>
-      <c r="B31" s="13"/>
-      <c r="C31" s="13"/>
-      <c r="D31" s="6" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" s="10" customFormat="1" ht="54.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="15"/>
-      <c r="B32" s="2"/>
-      <c r="C32" s="13"/>
-      <c r="D32" s="6" t="s">
+    <row r="26" spans="1:4" s="9" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="5"/>
+      <c r="B26" s="12"/>
+      <c r="C26" s="5"/>
+      <c r="D26" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" s="9" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="5"/>
+      <c r="B27" s="12"/>
+      <c r="C27" s="5"/>
+      <c r="D27" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="5"/>
+      <c r="B28" s="12"/>
+      <c r="C28" s="5"/>
+      <c r="D28" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="5"/>
+      <c r="B29" s="12"/>
+      <c r="C29" s="5"/>
+      <c r="D29" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" s="13" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="31" spans="1:4" s="9" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="14"/>
+      <c r="B31" s="12"/>
+      <c r="C31" s="12"/>
+      <c r="D31" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" s="9" customFormat="1" ht="54.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="14"/>
+      <c r="B32" s="1"/>
+      <c r="C32" s="12"/>
+      <c r="D32" s="5" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="33" spans="1:17" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="10"/>
-      <c r="C33" s="13"/>
-      <c r="D33" s="6" t="s">
+      <c r="A33" s="9"/>
+      <c r="C33" s="12"/>
+      <c r="D33" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="E33" s="10"/>
-      <c r="F33" s="10"/>
-      <c r="G33" s="10"/>
-      <c r="H33" s="10"/>
-      <c r="I33" s="10"/>
-      <c r="J33" s="10"/>
-      <c r="K33" s="10"/>
-      <c r="L33" s="10"/>
-      <c r="M33" s="10"/>
-      <c r="N33" s="10"/>
-      <c r="O33" s="10"/>
-      <c r="P33" s="10"/>
-      <c r="Q33" s="10"/>
+      <c r="E33" s="9"/>
+      <c r="F33" s="9"/>
+      <c r="G33" s="9"/>
+      <c r="H33" s="9"/>
+      <c r="I33" s="9"/>
+      <c r="J33" s="9"/>
+      <c r="K33" s="9"/>
+      <c r="L33" s="9"/>
+      <c r="M33" s="9"/>
+      <c r="N33" s="9"/>
+      <c r="O33" s="9"/>
+      <c r="P33" s="9"/>
+      <c r="Q33" s="9"/>
     </row>
     <row r="34" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
@@ -1017,7 +1065,7 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000000000000}">
           <x14:formula1>
             <xm:f>Sheet1!$A$1:$A$2</xm:f>
           </x14:formula1>
@@ -1026,7 +1074,7 @@
           </x14:formula2>
           <xm:sqref>D31:D33 D13:D29 D3:D4 D7:D11</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000001000000}">
           <x14:formula1>
             <xm:f>'[CDD_RL-1.xlsx]Sheet1'!#REF!</xm:f>
           </x14:formula1>
@@ -1042,25 +1090,25 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AMK2"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C12" activeCellId="2" sqref="A4:F4 G4 C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1025" width="8.7109375" style="10" customWidth="1"/>
+    <col min="1" max="1025" width="8.6640625" style="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A1" s="16" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A2" s="16" t="s">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" s="15" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" s="15" t="s">
         <v>20</v>
       </c>
     </row>

</xml_diff>